<commit_message>
fix: demo download + excel parser + example file link
Demo:
- Исправлен layout "classic" → "basic" в demo.py
- Добавлен endpoint /api/v1/demo/download/{file_id}
- Исправлен URL скачивания в demo-dropzone.tsx

Excel Parser:
- Добавлены колонки: brand, manufacturer, production_date, importer, certificate
- Обновлён wb-barcodes-example.xlsx с 12 колонками

Label Generator:
- Basic 58x40: 4 строки характеристик (цвет+размер, арт+страна, состав, бренд)
- Поднят текстовый блок выше от штрихкода

Frontend:
- Добавлена ссылка "Скачать пример Excel файла" в UnifiedDropzone

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/frontend/public/examples/wb-barcodes-example.xlsx
+++ b/frontend/public/examples/wb-barcodes-example.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Баркоды WB" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Товары" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -27,17 +27,24 @@
     </font>
     <font>
       <b val="1"/>
+      <sz val="10"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E8F5E9"/>
+        <bgColor rgb="00E8F5E9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,13 +52,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -417,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,13 +444,20 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="10" customWidth="1" min="3" max="3"/>
-    <col width="10" customWidth="1" min="4" max="4"/>
-    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="26" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="8" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="22" customWidth="1" min="7" max="7"/>
+    <col width="8" customWidth="1" min="8" max="8"/>
+    <col width="18" customWidth="1" min="9" max="9"/>
+    <col width="14" customWidth="1" min="10" max="10"/>
+    <col width="14" customWidth="1" min="11" max="11"/>
+    <col width="28" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="35" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Баркод</t>
@@ -440,157 +465,243 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Наименование</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Артикул</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Размер</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Цвет</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Наименование</t>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Бренд</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Состав</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Страна</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Производитель</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Дата производства</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Импортёр</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Сертификат</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>4601234567890</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>ABC-001</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Футболка женская хлопок</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>FTB-001</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>Белый</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Футболка хлопок</t>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>Nike</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>100% хлопок</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>Китай</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="inlineStr">
+        <is>
+          <t>ООО ТекстильПро</t>
+        </is>
+      </c>
+      <c r="J2" s="2" t="inlineStr">
+        <is>
+          <t>01.01.2026</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="inlineStr">
+        <is>
+          <t>ООО Импорт</t>
+        </is>
+      </c>
+      <c r="L2" s="2" t="inlineStr">
+        <is>
+          <t>ЕАЭС N RU Д-CN.АД65.В.01234/25</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>4601234567891</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ABC-001</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Футболка женская хлопок</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>FTB-001</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" s="2" t="inlineStr">
         <is>
           <t>Белый</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Футболка хлопок</t>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>Nike</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>100% хлопок</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="inlineStr">
+        <is>
+          <t>Китай</t>
+        </is>
+      </c>
+      <c r="I3" s="2" t="inlineStr">
+        <is>
+          <t>ООО ТекстильПро</t>
+        </is>
+      </c>
+      <c r="J3" s="2" t="inlineStr">
+        <is>
+          <t>01.01.2026</t>
+        </is>
+      </c>
+      <c r="K3" s="2" t="inlineStr">
+        <is>
+          <t>ООО Импорт</t>
+        </is>
+      </c>
+      <c r="L3" s="2" t="inlineStr">
+        <is>
+          <t>ЕАЭС N RU Д-CN.АД65.В.01234/25</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>4601234567892</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>ABC-001</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>L</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Белый</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Футболка хлопок</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4607654321098</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>XYZ-002</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>42</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Черный</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Джинсы slim</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>4607654321099</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>XYZ-002</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>44</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Черный</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Джинсы slim</t>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>Джинсы мужские классические</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>JNS-042</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>Синий</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>Levis</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>98% хлопок, 2% эластан</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="inlineStr">
+        <is>
+          <t>Турция</t>
+        </is>
+      </c>
+      <c r="I4" s="2" t="inlineStr">
+        <is>
+          <t>ИП Иванов И.И.</t>
+        </is>
+      </c>
+      <c r="J4" s="2" t="inlineStr">
+        <is>
+          <t>15.12.2025</t>
+        </is>
+      </c>
+      <c r="K4" s="2" t="inlineStr">
+        <is>
+          <t>ИП Иванов И.И.</t>
+        </is>
+      </c>
+      <c r="L4" s="2" t="inlineStr">
+        <is>
+          <t>РОСС RU.АВ71.Н12345</t>
         </is>
       </c>
     </row>

</xml_diff>